<commit_message>
Atualiza tabela CSV com resultados dos modelos
</commit_message>
<xml_diff>
--- a/tables/variaveis_utilizadas.xlsx
+++ b/tables/variaveis_utilizadas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="348">
   <si>
     <t xml:space="preserve">Variáveis utilizadas para treinamento dos modelos.</t>
   </si>
@@ -908,18 +908,6 @@
   </si>
   <si>
     <t xml:space="preserve">Quantidade de alunos com situação de vínculo no curso - matrícula trancada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QT_SIT_DESVINCULADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantidade de alunos com situação de vínculo no curso - aluno desvinculado do curso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QT_SIT_TRANSFERIDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantidade de alunos com situação de vínculo no curso - aluno transferido para outro curso da mesma IES</t>
   </si>
   <si>
     <t xml:space="preserve">QT_SIT_FALECIDO</t>
@@ -1090,6 +1078,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1111,12 +1100,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1166,7 +1157,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1191,13 +1182,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B179"/>
+  <dimension ref="A1:B177"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="141.21"/>
@@ -2596,22 +2587,6 @@
       </c>
       <c r="B177" s="0" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="B178" s="0" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="B179" s="0" t="s">
-        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>